<commit_message>
added bugfix barrage for TRY analysis in _process_specification
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/HP/data/deleteme.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/HP/data/deleteme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\HP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\HP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A428ED82-7F06-47A9-9084-6BAB43C4CC37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10805B9-69B1-4247-967D-2AC303B08525}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1716,14 +1716,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2127,1043 +2127,1043 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.16726605687524879</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>3.2087914536675637E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.6958267966010353</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.98758902426823802</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>2.2714547558169471</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>5.9717059986922769E-2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>6.1736692759945783E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.1235733067497632</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.21692155917850631</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>3.0242115788782159E-3</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.42410023855966539</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>1.573759840248915E-3</v>
       </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
         <v>1.573759840248915E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>0.1349652422667707</v>
       </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
         <v>0.2699304845335414</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>9.7261246972007484E-2</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
         <v>0.30021117997053282</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>2.5622363711604951E-2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.1653604483199819</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>5.8931436536691389E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>6.2641975711982059E-2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>2.191000463613172E-3</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>0.1465379713466696</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>1.97287496587335</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>1.2010706769697581</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>3.4955400563672052</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>4.7231957575180123</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>0.95944701655887232</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>8.1606042722821037</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>1.7100929821726749</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>2.3444256016165679</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>2.7361487714762802</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>0.72060303664359304</v>
       </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
         <v>1.297085465958467</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>11.253863219334271</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>1.2781595088798099</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>46.804654104301576</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>1.159154609780028</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>6.0366164537625902E-2</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>3.7199570106404751</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>0.48363107061413307</v>
       </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
         <v>2.0180855069048911</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>3.1889891554523269</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>2.6220016290209199E-2</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>13.49347646120993</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>0.12140770434282271</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>4.7392019975124558E-2</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>0.2063930973827986</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>0.82595871399553245</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>4.9461625776851377E-2</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>1.425252565493512</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>0.21639979884368951</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>9.8580625540908191E-3</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>0.33213475630907208</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>4.5012834484246924E-3</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>7.6936475180110653E-4</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>1.4854235379801481E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>6.0733195746984683E-3</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>3.2178644984612939E-3</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>2.004195459650495E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>4.823026839846924E-3</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>2.794387715909979E-3</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1.591598857149485E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>1.6675658149884299E-2</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>2.432061991716402E-2</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>5.5029671894618187E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>4.943446882298151E-3</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>1.570904852276037E-3</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>1.6313374711583901E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>4.823026839846924E-3</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>2.794387715909979E-3</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1.591598857149485E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>9.6397969060361147E-2</v>
       </c>
-      <c r="D31" s="3">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
         <v>0.30558156192134478</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>0.17050325274834349</v>
       </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
         <v>0.54049531121224892</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>5.1106208870099088E-3</v>
       </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
         <v>9.1991175966178364E-3</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>2.9389946330796109E-2</v>
       </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
         <v>9.3166129868623673E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>4.8024596643942562E-2</v>
       </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
         <v>0.15223797136129791</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>6.971551786408503E-2</v>
       </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36" s="3">
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
         <v>0.22099819162914949</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>4.5602941474980917E-2</v>
       </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
         <v>0.14456132447568951</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>0.38903842372368969</v>
       </c>
-      <c r="D38" s="3">
-        <v>0</v>
-      </c>
-      <c r="E38" s="3">
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
         <v>1.2136514212373331</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>0.2118956396982285</v>
       </c>
-      <c r="D39" s="3">
-        <v>0</v>
-      </c>
-      <c r="E39" s="3">
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
         <v>0.48735997130592551</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>1.8548462749368989E-2</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>3.085681739192217E-2</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>4.2661464323548677E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>1.627951626990215</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>4.632270974837098E-2</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>2.332672337714754</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>0.27358111794878232</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>3.4616208978161277E-2</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>0.82965176136236551</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>0.54036361287234114</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>5.1722352364024938E-3</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>1.4988882164654129</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>0.1404880999782705</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>3.15618528277012E-3</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>0.35861965491314562</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>0.35012266301331563</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>0.13931660104833041</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>0.65583899764905362</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>0.70265517643385944</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>0.14985647044328951</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>1.3678046926616101</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>20.83897523430258</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>2.8888667060229709</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>31.25846285145386</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>0.26092959739564792</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>4.3996439016896052E-2</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>0.48015927047281581</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>6.9446994166012573E-3</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>1.0209158586167451E-2</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>2.2917508074784151E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>4.6899352907091964E-3</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>1.1834652505916189E-3</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>1.5476786459340339E-2</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>9.8327463924684988</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>1.7787906856274491E-3</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>19.666683499404481</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>0.19073565839618489</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>2.486046175612881E-3</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>0.33971713765518657</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <v>0.72873862726131022</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>1.088251162487623E-2</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>1.41732640325098</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <v>0.27290831841080021</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="2">
         <v>8.0921365634117975E-2</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="2">
         <v>0.55400388637392428</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <v>1.1122401683114449E-2</v>
       </c>
-      <c r="D55" s="3">
-        <v>0</v>
-      </c>
-      <c r="E55" s="3">
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2">
         <v>2.9856439028073029E-2</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <v>3.3242184291470351E-3</v>
       </c>
-      <c r="D56" s="3">
-        <v>0</v>
-      </c>
-      <c r="E56" s="3">
+      <c r="D56" s="2">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2">
         <v>3.3242184291470351E-3</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="2">
         <v>0.1017767447387575</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="2">
         <v>2.0575015366359469E-4</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="2">
         <v>0.1585600615417298</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <v>0.45900244019158282</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="2">
         <v>1.72704975311306E-3</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="2">
         <v>0.72083706664030589</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="3">
-        <v>0</v>
-      </c>
-      <c r="D59" s="3">
-        <v>0</v>
-      </c>
-      <c r="E59" s="3">
+      <c r="C59" s="2">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <v>46.267576571200671</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="2">
         <v>3.467157750498274</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="2">
         <v>46.267576571200671</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C63" s="4" t="s">
+      <c r="B63" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="2">
         <v>41.81693887423306</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="2">
         <v>-50.590228019549059</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="2">
         <v>75.610075173644816</v>
       </c>
     </row>
@@ -3182,68 +3182,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -43721,28 +43721,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A2:E79"/>
+  <dimension ref="A2:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -43984,20 +43984,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -44126,20 +44126,20 @@
         <v>-6059.5826750587285</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -44242,17 +44242,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -44800,6 +44800,16 @@
       </c>
       <c r="D79">
         <v>439.77140417278957</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <f>SUM(C41:C79)</f>
+        <v>-67759.743545242382</v>
+      </c>
+      <c r="D80">
+        <f>SUM(D41:D79)</f>
+        <v>-4743.1820481669702</v>
       </c>
     </row>
   </sheetData>
@@ -44828,7 +44838,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -44842,7 +44852,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>380</v>
       </c>
@@ -44854,7 +44864,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>381</v>
       </c>
@@ -44889,7 +44899,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -44903,7 +44913,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>380</v>
       </c>
@@ -44915,7 +44925,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>386</v>
       </c>
@@ -44927,7 +44937,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>387</v>
       </c>
@@ -44936,7 +44946,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>388</v>
       </c>
@@ -44945,7 +44955,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>389</v>
       </c>
@@ -44957,7 +44967,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>390</v>
       </c>
@@ -44969,7 +44979,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>391</v>
       </c>
@@ -44981,7 +44991,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>392</v>
       </c>
@@ -45019,7 +45029,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -45033,7 +45043,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>380</v>
       </c>
@@ -45045,7 +45055,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>381</v>
       </c>
@@ -45094,7 +45104,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -45108,7 +45118,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>401</v>
       </c>
@@ -45120,7 +45130,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="1" t="s">
         <v>402</v>
       </c>
@@ -45158,7 +45168,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -45172,7 +45182,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
         <v>405</v>
       </c>
@@ -45302,7 +45312,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -45316,7 +45326,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="2"/>
+      <c r="A58" s="4"/>
       <c r="B58" s="1" t="s">
         <v>408</v>
       </c>
@@ -45328,7 +45338,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -45342,7 +45352,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
+      <c r="A60" s="4"/>
       <c r="B60" s="1" t="s">
         <v>410</v>
       </c>
@@ -45354,7 +45364,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="2"/>
+      <c r="A61" s="4"/>
       <c r="B61" s="1" t="s">
         <v>411</v>
       </c>
@@ -45366,7 +45376,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
+      <c r="A62" s="4"/>
       <c r="B62" s="1" t="s">
         <v>412</v>
       </c>
@@ -45378,7 +45388,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
+      <c r="A63" s="4"/>
       <c r="B63" s="1" t="s">
         <v>413</v>
       </c>
@@ -45416,7 +45426,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -45430,7 +45440,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
+      <c r="A69" s="4"/>
       <c r="B69" s="1" t="s">
         <v>404</v>
       </c>
@@ -45442,7 +45452,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="2"/>
+      <c r="A70" s="4"/>
       <c r="B70" s="1" t="s">
         <v>405</v>
       </c>
@@ -45480,7 +45490,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -45494,7 +45504,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="2"/>
+      <c r="A76" s="4"/>
       <c r="B76" s="1" t="s">
         <v>404</v>
       </c>
@@ -45506,7 +45516,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="2"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="1" t="s">
         <v>405</v>
       </c>
@@ -45544,7 +45554,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -45558,7 +45568,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
+      <c r="A83" s="4"/>
       <c r="B83" s="1" t="s">
         <v>416</v>
       </c>
@@ -45582,7 +45592,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -45596,7 +45606,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="2"/>
+      <c r="A88" s="4"/>
       <c r="B88" s="1" t="s">
         <v>418</v>
       </c>
@@ -45608,7 +45618,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="2"/>
+      <c r="A89" s="4"/>
       <c r="B89" s="1" t="s">
         <v>419</v>
       </c>
@@ -45620,7 +45630,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="2"/>
+      <c r="A90" s="4"/>
       <c r="B90" s="1" t="s">
         <v>420</v>
       </c>
@@ -45632,7 +45642,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -45646,7 +45656,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="2"/>
+      <c r="A92" s="4"/>
       <c r="B92" s="1" t="s">
         <v>422</v>
       </c>
@@ -45658,7 +45668,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="2"/>
+      <c r="A93" s="4"/>
       <c r="B93" s="1" t="s">
         <v>423</v>
       </c>
@@ -45670,7 +45680,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="2"/>
+      <c r="A94" s="4"/>
       <c r="B94" s="1" t="s">
         <v>424</v>
       </c>
@@ -45682,7 +45692,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="2"/>
+      <c r="A95" s="4"/>
       <c r="B95" s="1" t="s">
         <v>425</v>
       </c>
@@ -45694,7 +45704,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="2"/>
+      <c r="A96" s="4"/>
       <c r="B96" s="1" t="s">
         <v>426</v>
       </c>
@@ -45706,7 +45716,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="2"/>
+      <c r="A97" s="4"/>
       <c r="B97" s="1" t="s">
         <v>427</v>
       </c>
@@ -45718,7 +45728,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="2"/>
+      <c r="A98" s="4"/>
       <c r="B98" s="1" t="s">
         <v>428</v>
       </c>
@@ -45730,7 +45740,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
+      <c r="A99" s="4"/>
       <c r="B99" s="1" t="s">
         <v>429</v>
       </c>
@@ -45742,7 +45752,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="2"/>
+      <c r="A100" s="4"/>
       <c r="B100" s="1" t="s">
         <v>430</v>
       </c>
@@ -45754,7 +45764,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="2"/>
+      <c r="A101" s="4"/>
       <c r="B101" s="1" t="s">
         <v>431</v>
       </c>
@@ -45766,7 +45776,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="2"/>
+      <c r="A102" s="4"/>
       <c r="B102" s="1" t="s">
         <v>432</v>
       </c>
@@ -45778,7 +45788,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="2"/>
+      <c r="A103" s="4"/>
       <c r="B103" s="1" t="s">
         <v>433</v>
       </c>
@@ -45790,7 +45800,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="2"/>
+      <c r="A104" s="4"/>
       <c r="B104" s="1" t="s">
         <v>434</v>
       </c>
@@ -45802,7 +45812,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="2"/>
+      <c r="A105" s="4"/>
       <c r="B105" s="1" t="s">
         <v>435</v>
       </c>
@@ -45814,7 +45824,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="2"/>
+      <c r="A106" s="4"/>
       <c r="B106" s="1" t="s">
         <v>436</v>
       </c>
@@ -45918,7 +45928,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -45932,7 +45942,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="2"/>
+      <c r="A121" s="4"/>
       <c r="B121" s="1" t="s">
         <v>379</v>
       </c>
@@ -45944,7 +45954,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="2"/>
+      <c r="A122" s="4"/>
       <c r="B122" s="1" t="s">
         <v>380</v>
       </c>
@@ -45956,7 +45966,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="2"/>
+      <c r="A123" s="4"/>
       <c r="B123" s="1" t="s">
         <v>386</v>
       </c>
@@ -45968,7 +45978,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="2"/>
+      <c r="A124" s="4"/>
       <c r="B124" s="1" t="s">
         <v>387</v>
       </c>
@@ -45977,7 +45987,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="2"/>
+      <c r="A125" s="4"/>
       <c r="B125" s="1" t="s">
         <v>388</v>
       </c>
@@ -45986,7 +45996,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="2"/>
+      <c r="A126" s="4"/>
       <c r="B126" s="1" t="s">
         <v>389</v>
       </c>
@@ -45998,7 +46008,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="2"/>
+      <c r="A127" s="4"/>
       <c r="B127" s="1" t="s">
         <v>390</v>
       </c>
@@ -46010,7 +46020,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="2"/>
+      <c r="A128" s="4"/>
       <c r="B128" s="1" t="s">
         <v>391</v>
       </c>
@@ -46022,7 +46032,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="2"/>
+      <c r="A129" s="4"/>
       <c r="B129" s="1" t="s">
         <v>392</v>
       </c>
@@ -46034,7 +46044,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B130" s="1" t="s">
@@ -46048,7 +46058,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="2"/>
+      <c r="A131" s="4"/>
       <c r="B131" s="1" t="s">
         <v>407</v>
       </c>
@@ -46072,7 +46082,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -46086,7 +46096,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="2"/>
+      <c r="A136" s="4"/>
       <c r="B136" s="1" t="s">
         <v>380</v>
       </c>
@@ -46098,7 +46108,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="2"/>
+      <c r="A137" s="4"/>
       <c r="B137" s="1" t="s">
         <v>386</v>
       </c>
@@ -46110,7 +46120,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="2"/>
+      <c r="A138" s="4"/>
       <c r="B138" s="1" t="s">
         <v>387</v>
       </c>
@@ -46119,7 +46129,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="2"/>
+      <c r="A139" s="4"/>
       <c r="B139" s="1" t="s">
         <v>388</v>
       </c>
@@ -46128,7 +46138,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="2"/>
+      <c r="A140" s="4"/>
       <c r="B140" s="1" t="s">
         <v>389</v>
       </c>
@@ -46140,7 +46150,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" s="2"/>
+      <c r="A141" s="4"/>
       <c r="B141" s="1" t="s">
         <v>390</v>
       </c>
@@ -46152,7 +46162,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="2"/>
+      <c r="A142" s="4"/>
       <c r="B142" s="1" t="s">
         <v>391</v>
       </c>
@@ -46164,7 +46174,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" s="2"/>
+      <c r="A143" s="4"/>
       <c r="B143" s="1" t="s">
         <v>392</v>
       </c>
@@ -46176,7 +46186,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B144" s="1" t="s">
@@ -46190,7 +46200,7 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145" s="2"/>
+      <c r="A145" s="4"/>
       <c r="B145" s="1" t="s">
         <v>440</v>
       </c>
@@ -46202,7 +46212,7 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" s="2"/>
+      <c r="A146" s="4"/>
       <c r="B146" s="1" t="s">
         <v>441</v>
       </c>
@@ -46229,7 +46239,7 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B150" s="1" t="s">
@@ -46243,7 +46253,7 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" s="2"/>
+      <c r="A151" s="4"/>
       <c r="B151" s="1" t="s">
         <v>443</v>
       </c>
@@ -46255,7 +46265,7 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="2"/>
+      <c r="A152" s="4"/>
       <c r="B152" s="1" t="s">
         <v>444</v>
       </c>
@@ -46270,7 +46280,7 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A153" s="2"/>
+      <c r="A153" s="4"/>
       <c r="B153" s="1" t="s">
         <v>445</v>
       </c>
@@ -46285,7 +46295,7 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A154" s="2"/>
+      <c r="A154" s="4"/>
       <c r="B154" s="1" t="s">
         <v>446</v>
       </c>
@@ -46297,7 +46307,7 @@
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" s="2"/>
+      <c r="A155" s="4"/>
       <c r="B155" s="1" t="s">
         <v>447</v>
       </c>
@@ -46309,7 +46319,7 @@
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" s="2"/>
+      <c r="A156" s="4"/>
       <c r="B156" s="1" t="s">
         <v>448</v>
       </c>
@@ -46324,7 +46334,7 @@
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" s="2"/>
+      <c r="A157" s="4"/>
       <c r="B157" s="1" t="s">
         <v>449</v>
       </c>
@@ -46339,7 +46349,7 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" s="2"/>
+      <c r="A158" s="4"/>
       <c r="B158" s="1" t="s">
         <v>450</v>
       </c>
@@ -46354,7 +46364,7 @@
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" s="2"/>
+      <c r="A159" s="4"/>
       <c r="B159" s="1" t="s">
         <v>451</v>
       </c>
@@ -46369,7 +46379,7 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" s="2"/>
+      <c r="A160" s="4"/>
       <c r="B160" s="1" t="s">
         <v>452</v>
       </c>
@@ -46384,7 +46394,7 @@
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" s="2"/>
+      <c r="A161" s="4"/>
       <c r="B161" s="1" t="s">
         <v>453</v>
       </c>
@@ -46399,7 +46409,7 @@
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A162" s="2"/>
+      <c r="A162" s="4"/>
       <c r="B162" s="1" t="s">
         <v>454</v>
       </c>
@@ -46414,7 +46424,7 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A163" s="2"/>
+      <c r="A163" s="4"/>
       <c r="B163" s="1" t="s">
         <v>455</v>
       </c>
@@ -46429,7 +46439,7 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A164" s="2" t="s">
+      <c r="A164" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -46446,7 +46456,7 @@
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A165" s="2"/>
+      <c r="A165" s="4"/>
       <c r="B165" s="1" t="s">
         <v>457</v>
       </c>
@@ -46461,7 +46471,7 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A166" s="2"/>
+      <c r="A166" s="4"/>
       <c r="B166" s="1" t="s">
         <v>458</v>
       </c>
@@ -46476,7 +46486,7 @@
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A167" s="2"/>
+      <c r="A167" s="4"/>
       <c r="B167" s="1" t="s">
         <v>459</v>
       </c>
@@ -46491,7 +46501,7 @@
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A168" s="2"/>
+      <c r="A168" s="4"/>
       <c r="B168" s="1" t="s">
         <v>460</v>
       </c>
@@ -46503,7 +46513,7 @@
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A169" s="2"/>
+      <c r="A169" s="4"/>
       <c r="B169" s="1" t="s">
         <v>461</v>
       </c>
@@ -46518,7 +46528,7 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A170" s="2"/>
+      <c r="A170" s="4"/>
       <c r="B170" s="1" t="s">
         <v>413</v>
       </c>
@@ -46639,7 +46649,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" s="2" t="s">
+      <c r="A185" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B185" s="1" t="s">
@@ -46653,7 +46663,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" s="2"/>
+      <c r="A186" s="4"/>
       <c r="B186" s="1" t="s">
         <v>405</v>
       </c>
@@ -46677,7 +46687,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B190" s="1" t="s">
@@ -46691,7 +46701,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" s="2"/>
+      <c r="A191" s="4"/>
       <c r="B191" s="1" t="s">
         <v>420</v>
       </c>
@@ -46703,7 +46713,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -46717,7 +46727,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A193" s="2"/>
+      <c r="A193" s="4"/>
       <c r="B193" s="1" t="s">
         <v>465</v>
       </c>
@@ -46756,7 +46766,7 @@
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A197" s="2" t="s">
+      <c r="A197" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -46785,7 +46795,7 @@
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A198" s="2"/>
+      <c r="A198" s="4"/>
       <c r="B198" s="1" t="s">
         <v>399</v>
       </c>
@@ -46812,7 +46822,7 @@
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" s="2"/>
+      <c r="A199" s="4"/>
       <c r="B199" s="1" t="s">
         <v>467</v>
       </c>
@@ -46836,7 +46846,7 @@
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A200" s="2"/>
+      <c r="A200" s="4"/>
       <c r="B200" s="1" t="s">
         <v>468</v>
       </c>
@@ -46860,7 +46870,7 @@
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A201" s="2"/>
+      <c r="A201" s="4"/>
       <c r="B201" s="1" t="s">
         <v>469</v>
       </c>
@@ -46884,7 +46894,7 @@
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" s="2"/>
+      <c r="A202" s="4"/>
       <c r="B202" s="1" t="s">
         <v>470</v>
       </c>
@@ -46908,7 +46918,7 @@
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A203" s="2"/>
+      <c r="A203" s="4"/>
       <c r="B203" s="1" t="s">
         <v>471</v>
       </c>
@@ -46935,7 +46945,7 @@
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A204" s="2"/>
+      <c r="A204" s="4"/>
       <c r="B204" s="1" t="s">
         <v>472</v>
       </c>
@@ -46959,7 +46969,7 @@
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A205" s="2" t="s">
+      <c r="A205" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -46988,7 +46998,7 @@
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A206" s="2"/>
+      <c r="A206" s="4"/>
       <c r="B206" s="1" t="s">
         <v>473</v>
       </c>
@@ -47045,7 +47055,7 @@
       </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A210" s="2" t="s">
+      <c r="A210" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B210" s="1" t="s">
@@ -47077,7 +47087,7 @@
       </c>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A211" s="2"/>
+      <c r="A211" s="4"/>
       <c r="B211" s="1" t="s">
         <v>478</v>
       </c>
@@ -47107,7 +47117,7 @@
       </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A212" s="2"/>
+      <c r="A212" s="4"/>
       <c r="B212" s="1" t="s">
         <v>479</v>
       </c>
@@ -47137,7 +47147,7 @@
       </c>
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A213" s="2"/>
+      <c r="A213" s="4"/>
       <c r="B213" s="1" t="s">
         <v>480</v>
       </c>
@@ -47164,7 +47174,7 @@
       </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A214" s="2"/>
+      <c r="A214" s="4"/>
       <c r="B214" s="1" t="s">
         <v>481</v>
       </c>
@@ -47194,7 +47204,7 @@
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A215" s="2"/>
+      <c r="A215" s="4"/>
       <c r="B215" s="1" t="s">
         <v>482</v>
       </c>
@@ -47224,7 +47234,7 @@
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A216" s="2"/>
+      <c r="A216" s="4"/>
       <c r="B216" s="1" t="s">
         <v>483</v>
       </c>
@@ -47254,7 +47264,7 @@
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A217" s="2"/>
+      <c r="A217" s="4"/>
       <c r="B217" s="1" t="s">
         <v>484</v>
       </c>
@@ -47354,7 +47364,7 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A226" s="2" t="s">
+      <c r="A226" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -47368,7 +47378,7 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A227" s="2"/>
+      <c r="A227" s="4"/>
       <c r="B227" s="1" t="s">
         <v>380</v>
       </c>
@@ -47380,7 +47390,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A228" s="2"/>
+      <c r="A228" s="4"/>
       <c r="B228" s="1" t="s">
         <v>381</v>
       </c>
@@ -47469,7 +47479,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A239" s="2" t="s">
+      <c r="A239" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B239" s="1" t="s">
@@ -47483,7 +47493,7 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A240" s="2"/>
+      <c r="A240" s="4"/>
       <c r="B240" s="1" t="s">
         <v>490</v>
       </c>
@@ -47495,7 +47505,7 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A241" s="2"/>
+      <c r="A241" s="4"/>
       <c r="B241" s="1" t="s">
         <v>491</v>
       </c>
@@ -47507,7 +47517,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A242" s="2"/>
+      <c r="A242" s="4"/>
       <c r="B242" s="1" t="s">
         <v>492</v>
       </c>
@@ -47531,7 +47541,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A246" s="2" t="s">
+      <c r="A246" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B246" s="1" t="s">
@@ -47545,7 +47555,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A247" s="2"/>
+      <c r="A247" s="4"/>
       <c r="B247" s="1" t="s">
         <v>494</v>
       </c>
@@ -47557,7 +47567,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A248" s="2"/>
+      <c r="A248" s="4"/>
       <c r="B248" s="1" t="s">
         <v>495</v>
       </c>
@@ -47566,7 +47576,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A249" s="2"/>
+      <c r="A249" s="4"/>
       <c r="B249" s="1" t="s">
         <v>496</v>
       </c>
@@ -47578,7 +47588,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A250" s="2"/>
+      <c r="A250" s="4"/>
       <c r="B250" s="1" t="s">
         <v>497</v>
       </c>
@@ -47590,7 +47600,7 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A251" s="2"/>
+      <c r="A251" s="4"/>
       <c r="B251" s="1" t="s">
         <v>498</v>
       </c>
@@ -47602,7 +47612,7 @@
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A252" s="2"/>
+      <c r="A252" s="4"/>
       <c r="B252" s="1" t="s">
         <v>499</v>
       </c>
@@ -47614,7 +47624,7 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A253" s="2"/>
+      <c r="A253" s="4"/>
       <c r="B253" s="1" t="s">
         <v>500</v>
       </c>
@@ -47623,7 +47633,7 @@
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A254" s="2"/>
+      <c r="A254" s="4"/>
       <c r="B254" s="1" t="s">
         <v>501</v>
       </c>
@@ -47635,7 +47645,7 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A255" s="2"/>
+      <c r="A255" s="4"/>
       <c r="B255" s="1" t="s">
         <v>502</v>
       </c>
@@ -47647,7 +47657,7 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A256" s="2"/>
+      <c r="A256" s="4"/>
       <c r="B256" s="1" t="s">
         <v>503</v>
       </c>
@@ -47659,7 +47669,7 @@
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A257" s="2"/>
+      <c r="A257" s="4"/>
       <c r="B257" s="1" t="s">
         <v>504</v>
       </c>
@@ -47671,7 +47681,7 @@
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A258" s="2"/>
+      <c r="A258" s="4"/>
       <c r="B258" s="1" t="s">
         <v>505</v>
       </c>
@@ -47680,7 +47690,7 @@
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A259" s="2" t="s">
+      <c r="A259" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B259" s="1" t="s">
@@ -47694,7 +47704,7 @@
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A260" s="2"/>
+      <c r="A260" s="4"/>
       <c r="B260" s="1" t="s">
         <v>507</v>
       </c>
@@ -47721,7 +47731,7 @@
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A264" s="2" t="s">
+      <c r="A264" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B264" s="1" t="s">
@@ -47738,7 +47748,7 @@
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A265" s="2"/>
+      <c r="A265" s="4"/>
       <c r="B265" s="1" t="s">
         <v>509</v>
       </c>
@@ -47753,7 +47763,7 @@
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A266" s="2" t="s">
+      <c r="A266" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B266" s="1" t="s">
@@ -47770,7 +47780,7 @@
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A267" s="2"/>
+      <c r="A267" s="4"/>
       <c r="B267" s="1" t="s">
         <v>510</v>
       </c>
@@ -47785,7 +47795,7 @@
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A268" s="2"/>
+      <c r="A268" s="4"/>
       <c r="B268" s="1" t="s">
         <v>511</v>
       </c>
@@ -47826,7 +47836,7 @@
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A273" s="2" t="s">
+      <c r="A273" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B273" s="1" t="s">
@@ -47840,7 +47850,7 @@
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A274" s="2"/>
+      <c r="A274" s="4"/>
       <c r="B274" s="1" t="s">
         <v>404</v>
       </c>
@@ -47852,7 +47862,7 @@
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A275" s="2"/>
+      <c r="A275" s="4"/>
       <c r="B275" s="1" t="s">
         <v>405</v>
       </c>
@@ -47876,7 +47886,7 @@
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A279" s="2" t="s">
+      <c r="A279" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B279" s="1" t="s">
@@ -47890,7 +47900,7 @@
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A280" s="2"/>
+      <c r="A280" s="4"/>
       <c r="B280" s="1" t="s">
         <v>514</v>
       </c>
@@ -47899,7 +47909,7 @@
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A281" s="2" t="s">
+      <c r="A281" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B281" s="1" t="s">
@@ -47913,7 +47923,7 @@
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A282" s="2"/>
+      <c r="A282" s="4"/>
       <c r="B282" s="1" t="s">
         <v>404</v>
       </c>
@@ -47925,7 +47935,7 @@
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A283" s="2"/>
+      <c r="A283" s="4"/>
       <c r="B283" s="1" t="s">
         <v>405</v>
       </c>
@@ -47937,7 +47947,7 @@
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A284" s="2"/>
+      <c r="A284" s="4"/>
       <c r="B284" s="1" t="s">
         <v>407</v>
       </c>
@@ -48015,7 +48025,7 @@
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A294" s="2" t="s">
+      <c r="A294" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B294" s="1" t="s">
@@ -48029,7 +48039,7 @@
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A295" s="2"/>
+      <c r="A295" s="4"/>
       <c r="B295" s="1" t="s">
         <v>519</v>
       </c>
@@ -48041,7 +48051,7 @@
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A296" s="2"/>
+      <c r="A296" s="4"/>
       <c r="B296" s="1" t="s">
         <v>405</v>
       </c>
@@ -48068,7 +48078,7 @@
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A300" s="2" t="s">
+      <c r="A300" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B300" s="1" t="s">
@@ -48085,7 +48095,7 @@
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A301" s="2"/>
+      <c r="A301" s="4"/>
       <c r="B301" s="1" t="s">
         <v>399</v>
       </c>
@@ -48100,7 +48110,7 @@
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A302" s="2"/>
+      <c r="A302" s="4"/>
       <c r="B302" s="1" t="s">
         <v>467</v>
       </c>
@@ -48112,7 +48122,7 @@
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A303" s="2"/>
+      <c r="A303" s="4"/>
       <c r="B303" s="1" t="s">
         <v>468</v>
       </c>
@@ -48124,7 +48134,7 @@
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A304" s="2"/>
+      <c r="A304" s="4"/>
       <c r="B304" s="1" t="s">
         <v>469</v>
       </c>
@@ -48136,7 +48146,7 @@
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A305" s="2"/>
+      <c r="A305" s="4"/>
       <c r="B305" s="1" t="s">
         <v>470</v>
       </c>
@@ -48148,7 +48158,7 @@
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A306" s="2"/>
+      <c r="A306" s="4"/>
       <c r="B306" s="1" t="s">
         <v>471</v>
       </c>
@@ -48163,7 +48173,7 @@
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A307" s="2"/>
+      <c r="A307" s="4"/>
       <c r="B307" s="1" t="s">
         <v>472</v>
       </c>
@@ -48175,7 +48185,7 @@
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A308" s="2" t="s">
+      <c r="A308" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B308" s="1" t="s">
@@ -48192,7 +48202,7 @@
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A309" s="2"/>
+      <c r="A309" s="4"/>
       <c r="B309" s="1" t="s">
         <v>473</v>
       </c>
@@ -48219,7 +48229,7 @@
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A313" s="2" t="s">
+      <c r="A313" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B313" s="1" t="s">
@@ -48233,7 +48243,7 @@
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A314" s="2"/>
+      <c r="A314" s="4"/>
       <c r="B314" s="1" t="s">
         <v>521</v>
       </c>
@@ -48245,7 +48255,7 @@
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A315" s="2" t="s">
+      <c r="A315" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B315" s="1" t="s">
@@ -48259,7 +48269,7 @@
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A316" s="2"/>
+      <c r="A316" s="4"/>
       <c r="B316" s="1" t="s">
         <v>523</v>
       </c>
@@ -48297,7 +48307,7 @@
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A321" s="2" t="s">
+      <c r="A321" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B321" s="1" t="s">
@@ -48311,7 +48321,7 @@
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A322" s="2"/>
+      <c r="A322" s="4"/>
       <c r="B322" s="1" t="s">
         <v>404</v>
       </c>
@@ -48323,7 +48333,7 @@
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A323" s="2"/>
+      <c r="A323" s="4"/>
       <c r="B323" s="1" t="s">
         <v>405</v>
       </c>
@@ -48347,7 +48357,7 @@
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A327" s="2" t="s">
+      <c r="A327" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B327" s="1" t="s">
@@ -48361,7 +48371,7 @@
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A328" s="2"/>
+      <c r="A328" s="4"/>
       <c r="B328" s="1" t="s">
         <v>525</v>
       </c>
@@ -48373,7 +48383,7 @@
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A329" s="2" t="s">
+      <c r="A329" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B329" s="1" t="s">
@@ -48387,7 +48397,7 @@
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A330" s="2"/>
+      <c r="A330" s="4"/>
       <c r="B330" s="1" t="s">
         <v>527</v>
       </c>
@@ -48399,7 +48409,7 @@
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A331" s="2"/>
+      <c r="A331" s="4"/>
       <c r="B331" s="1" t="s">
         <v>528</v>
       </c>
@@ -48411,7 +48421,7 @@
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A332" s="2"/>
+      <c r="A332" s="4"/>
       <c r="B332" s="1" t="s">
         <v>529</v>
       </c>
@@ -48423,7 +48433,7 @@
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A333" s="2"/>
+      <c r="A333" s="4"/>
       <c r="B333" s="1" t="s">
         <v>530</v>
       </c>
@@ -48435,7 +48445,7 @@
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A334" s="2"/>
+      <c r="A334" s="4"/>
       <c r="B334" s="1" t="s">
         <v>531</v>
       </c>
@@ -48447,7 +48457,7 @@
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A335" s="2"/>
+      <c r="A335" s="4"/>
       <c r="B335" s="1" t="s">
         <v>532</v>
       </c>
@@ -48459,7 +48469,7 @@
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A336" s="2"/>
+      <c r="A336" s="4"/>
       <c r="B336" s="1" t="s">
         <v>533</v>
       </c>
@@ -48483,7 +48493,7 @@
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A340" s="2" t="s">
+      <c r="A340" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B340" s="1" t="s">
@@ -48497,7 +48507,7 @@
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A341" s="2"/>
+      <c r="A341" s="4"/>
       <c r="B341" s="1" t="s">
         <v>399</v>
       </c>
@@ -48509,7 +48519,7 @@
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A342" s="2"/>
+      <c r="A342" s="4"/>
       <c r="B342" s="1" t="s">
         <v>535</v>
       </c>
@@ -48558,7 +48568,7 @@
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A348" s="2" t="s">
+      <c r="A348" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B348" s="1" t="s">
@@ -48572,7 +48582,7 @@
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A349" s="2"/>
+      <c r="A349" s="4"/>
       <c r="B349" s="1" t="s">
         <v>405</v>
       </c>
@@ -48656,7 +48666,7 @@
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A359" s="2" t="s">
+      <c r="A359" s="4" t="s">
         <v>378</v>
       </c>
       <c r="B359" s="1" t="s">
@@ -48673,7 +48683,7 @@
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A360" s="2"/>
+      <c r="A360" s="4"/>
       <c r="B360" s="1" t="s">
         <v>405</v>
       </c>
@@ -48700,7 +48710,7 @@
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A364" s="2" t="s">
+      <c r="A364" s="4" t="s">
         <v>377</v>
       </c>
       <c r="B364" s="1" t="s">
@@ -48714,7 +48724,7 @@
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A365" s="2"/>
+      <c r="A365" s="4"/>
       <c r="B365" s="1" t="s">
         <v>380</v>
       </c>
@@ -48726,7 +48736,7 @@
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A366" s="2"/>
+      <c r="A366" s="4"/>
       <c r="B366" s="1" t="s">
         <v>381</v>
       </c>
@@ -48790,51 +48800,51 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A106"/>
+    <mergeCell ref="A120:A129"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="A135:A143"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="A150:A163"/>
+    <mergeCell ref="A164:A170"/>
+    <mergeCell ref="A185:A186"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A197:A204"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A210:A217"/>
+    <mergeCell ref="A226:A228"/>
+    <mergeCell ref="A239:A242"/>
+    <mergeCell ref="A246:A258"/>
+    <mergeCell ref="A259:A260"/>
+    <mergeCell ref="A264:A265"/>
+    <mergeCell ref="A266:A268"/>
+    <mergeCell ref="A273:A275"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="A281:A284"/>
+    <mergeCell ref="A294:A296"/>
+    <mergeCell ref="A300:A307"/>
+    <mergeCell ref="A308:A309"/>
+    <mergeCell ref="A313:A314"/>
+    <mergeCell ref="A315:A316"/>
+    <mergeCell ref="A321:A323"/>
+    <mergeCell ref="A327:A328"/>
     <mergeCell ref="A329:A336"/>
     <mergeCell ref="A340:A342"/>
     <mergeCell ref="A348:A349"/>
     <mergeCell ref="A359:A360"/>
     <mergeCell ref="A364:A366"/>
-    <mergeCell ref="A308:A309"/>
-    <mergeCell ref="A313:A314"/>
-    <mergeCell ref="A315:A316"/>
-    <mergeCell ref="A321:A323"/>
-    <mergeCell ref="A327:A328"/>
-    <mergeCell ref="A273:A275"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="A281:A284"/>
-    <mergeCell ref="A294:A296"/>
-    <mergeCell ref="A300:A307"/>
-    <mergeCell ref="A239:A242"/>
-    <mergeCell ref="A246:A258"/>
-    <mergeCell ref="A259:A260"/>
-    <mergeCell ref="A264:A265"/>
-    <mergeCell ref="A266:A268"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="A197:A204"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A210:A217"/>
-    <mergeCell ref="A226:A228"/>
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="A150:A163"/>
-    <mergeCell ref="A164:A170"/>
-    <mergeCell ref="A185:A186"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A106"/>
-    <mergeCell ref="A120:A129"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="A135:A143"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A10:A18"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>